<commit_message>
explicit consent to data privacy note and ToU
</commit_message>
<xml_diff>
--- a/ScopingReview_4.xlsx
+++ b/ScopingReview_4.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mueller_admin.ZPIDNB21\Documents\Desktop\Rprojects\Scoping-Review\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C5D33EE-9B01-4469-8459-05110E9BA8E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F99CA30A-D61C-4279-89C7-7DC65DD9237A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Titlepage" sheetId="1" r:id="rId1"/>
@@ -485,9 +485,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -984,7 +985,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:L14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A8" sqref="A8:XFD8"/>
     </sheetView>
   </sheetViews>
@@ -1748,8 +1749,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:L4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1842,7 +1843,7 @@
       <c r="D4" t="s">
         <v>13</v>
       </c>
-      <c r="I4" t="s">
+      <c r="I4" s="2" t="s">
         <v>128</v>
       </c>
       <c r="K4" t="s">

</xml_diff>